<commit_message>
update point based system to README
</commit_message>
<xml_diff>
--- a/Facters_of_infections.xlsx
+++ b/Facters_of_infections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\github\tmcovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5ADDBE-7921-47DC-8D53-BF2C34F4BDE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60974A49-C067-4D56-B328-1170A45FFC7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5832" yWindow="2244" windowWidth="22344" windowHeight="12708" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="83">
   <si>
     <t>Inputs</t>
   </si>
@@ -371,7 +371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -576,6 +576,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -755,9 +775,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -790,9 +807,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -810,6 +824,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2168,44 +2188,44 @@
   <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5546875" defaultRowHeight="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="79"/>
-    <col min="2" max="2" width="19.77734375" style="79" customWidth="1"/>
-    <col min="3" max="4" width="16.5546875" style="79"/>
-    <col min="5" max="5" width="15.77734375" style="79" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="79"/>
-    <col min="7" max="8" width="15.5546875" style="79" customWidth="1"/>
-    <col min="9" max="16384" width="16.5546875" style="79"/>
+    <col min="1" max="1" width="16.5546875" style="77"/>
+    <col min="2" max="2" width="19.77734375" style="77" customWidth="1"/>
+    <col min="3" max="4" width="16.5546875" style="77"/>
+    <col min="5" max="5" width="15.77734375" style="77" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="77"/>
+    <col min="7" max="8" width="15.5546875" style="77" customWidth="1"/>
+    <col min="9" max="16384" width="16.5546875" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="G2" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="65" t="s">
+      <c r="H2" s="64" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="65" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="56"/>
@@ -2221,10 +2241,10 @@
       <c r="G3" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="67"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="68"/>
+      <c r="B4" s="67"/>
       <c r="C4" s="58" t="s">
         <v>53</v>
       </c>
@@ -2240,10 +2260,10 @@
       <c r="G4" s="58">
         <v>12</v>
       </c>
-      <c r="H4" s="67"/>
+      <c r="H4" s="66"/>
     </row>
     <row r="5" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="65" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="56"/>
@@ -2259,10 +2279,10 @@
       <c r="G5" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="69"/>
+      <c r="H5" s="68"/>
     </row>
     <row r="6" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="58" t="s">
         <v>53</v>
       </c>
@@ -2278,10 +2298,10 @@
       <c r="G6" s="58">
         <v>10</v>
       </c>
-      <c r="H6" s="69"/>
+      <c r="H6" s="68"/>
     </row>
     <row r="7" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="65" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="56"/>
@@ -2295,10 +2315,10 @@
         <v>18</v>
       </c>
       <c r="G7" s="59"/>
-      <c r="H7" s="69"/>
+      <c r="H7" s="68"/>
     </row>
     <row r="8" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="68"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="58" t="s">
         <v>53</v>
       </c>
@@ -2312,10 +2332,10 @@
         <v>6</v>
       </c>
       <c r="G8" s="59"/>
-      <c r="H8" s="69"/>
+      <c r="H8" s="68"/>
     </row>
     <row r="9" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="65" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="56"/>
@@ -2331,12 +2351,12 @@
       <c r="G9" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="70" t="s">
+      <c r="H9" s="69" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="58" t="s">
         <v>53</v>
       </c>
@@ -2352,93 +2372,107 @@
       <c r="G10" s="58">
         <v>6</v>
       </c>
-      <c r="H10" s="71">
+      <c r="H10" s="70">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="72"/>
+      <c r="B11" s="65" t="s">
+        <v>29</v>
+      </c>
       <c r="C11" s="56"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="73"/>
-    </row>
-    <row r="12" spans="2:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="57" t="s">
+      <c r="D11" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E11" s="57" t="s">
         <v>32</v>
+      </c>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="66"/>
+    </row>
+    <row r="12" spans="2:12" s="56" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="71"/>
+      <c r="C12" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="58">
+        <v>3</v>
+      </c>
+      <c r="E12" s="58">
+        <v>1</v>
       </c>
       <c r="F12" s="59"/>
       <c r="G12" s="59"/>
-      <c r="H12" s="67"/>
+      <c r="H12" s="68"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="78">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="2:12" s="56" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="72"/>
-      <c r="C13" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="58">
-        <v>3</v>
-      </c>
-      <c r="E13" s="58">
-        <v>1</v>
-      </c>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="69"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80">
-        <v>3</v>
-      </c>
+      <c r="B13" s="79" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="80"/>
+      <c r="D13" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
     </row>
     <row r="14" spans="2:12" s="56" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="61" t="s">
+      <c r="E14" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="61" t="s">
+      <c r="F14" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="74" t="s">
+      <c r="G14" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="80"/>
-      <c r="L14" s="80"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
     </row>
     <row r="15" spans="2:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="75"/>
-      <c r="C15" s="76" t="s">
+      <c r="B15" s="73"/>
+      <c r="C15" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="76" t="s">
+      <c r="D15" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="76" t="s">
+      <c r="F15" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="76" t="s">
+      <c r="G15" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="78" t="s">
+      <c r="H15" s="76" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>